<commit_message>
made modifications to drivetrain calc
</commit_message>
<xml_diff>
--- a/hardware/drive_calculations/drivetrain_calculations.xlsx
+++ b/hardware/drive_calculations/drivetrain_calculations.xlsx
@@ -3,7 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Drivetrain_Calc" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="V_RPM" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Inputs</t>
   </si>
@@ -76,32 +77,50 @@
     <t>Capacity (mAh)</t>
   </si>
   <si>
-    <t>Battery Discharge current (mAh)</t>
+    <t>Max Cont. Current</t>
   </si>
   <si>
     <t>Battery info</t>
   </si>
   <si>
+    <t>Current Drawn (A)</t>
+  </si>
+  <si>
+    <t>MCU (ESP-32)</t>
+  </si>
+  <si>
+    <t>Gyro (MPU-6050)</t>
+  </si>
+  <si>
+    <t>Motor Driver (logic)</t>
+  </si>
+  <si>
     <t>Total Current Draw</t>
   </si>
   <si>
     <t>Runtime (h)</t>
   </si>
   <si>
-    <t xml:space="preserve">Power </t>
+    <t>Power Info</t>
   </si>
   <si>
     <t>desired speed(m/s)</t>
   </si>
   <si>
     <t>desired max acceleration(m/s^2)</t>
+  </si>
+  <si>
+    <t>Supply Voltage</t>
+  </si>
+  <si>
+    <t>RPM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -140,6 +159,7 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font/>
   </fonts>
   <fills count="4">
     <fill>
@@ -161,12 +181,42 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -181,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -195,16 +245,39 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -216,6 +289,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -427,7 +504,7 @@
     <col customWidth="1" min="2" max="2" width="24.88"/>
     <col customWidth="1" min="3" max="3" width="25.0"/>
     <col customWidth="1" min="4" max="4" width="26.75"/>
-    <col customWidth="1" min="5" max="5" width="11.25"/>
+    <col customWidth="1" min="5" max="6" width="15.88"/>
     <col customWidth="1" min="7" max="7" width="19.75"/>
     <col customWidth="1" min="8" max="8" width="13.63"/>
   </cols>
@@ -457,226 +534,317 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>0.8</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="8">
         <v>1.5</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="8">
         <v>12.0</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7">
-        <f>C4*C15*(B6/2)*2</f>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9">
+        <f>C4*C17*(B6/2)*2</f>
         <v>0.15</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="9">
         <f>B4*C4*9.81</f>
         <v>11.772</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>0.1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="8">
         <v>2.0</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>12.0</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="8">
         <v>1.0</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="8">
         <v>200.0</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="8">
         <v>2.0</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="10">
         <f>16*0.0981</f>
         <v>1.5696</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="8">
         <v>10.0</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="9">
         <f>PI()*B6*(D8/60)</f>
         <v>1.047197551</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="4"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7">
-        <f>(B10*1000)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="B10" s="8">
+        <v>30.0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>850.0</v>
+      </c>
+      <c r="D10" s="9">
+        <f>B10*(C10/1000)</f>
+        <v>25.5</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="9"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="15"/>
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10" t="str">
-        <f>C10/B12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="9"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="D13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="7"/>
     </row>
     <row r="14">
-      <c r="A14" s="9"/>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="4"/>
+      <c r="A14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.005</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="16">
+        <f>B14+C14+D14+C8*E8</f>
+        <v>2.155</v>
+      </c>
+      <c r="G14" s="16">
+        <f>C10/F14</f>
+        <v>394.4315545</v>
+      </c>
+      <c r="H14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="9"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6">
+      <c r="A15" s="11"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="11"/>
+      <c r="B16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="11"/>
+      <c r="B17" s="8">
         <v>1.0</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="C17" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B12:D12"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="17">
+        <v>3.0</v>
+      </c>
+      <c r="B2" s="17">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="17">
+        <v>6.0</v>
+      </c>
+      <c r="B3" s="17">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="17">
+        <v>12.0</v>
+      </c>
+      <c r="B4" s="17">
+        <v>200.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>